<commit_message>
Removed leading space on parameter
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GSA\GSA_GIT\piv-conformance-swing\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5D85D1-4438-4497-96B6-A7473503BAE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47202FC2-972A-4DC6-849C-57E9C0B0C831}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="1995" windowWidth="28410" windowHeight="14550" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="1265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3646" uniqueCount="1267">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3828,6 +3828,12 @@
   </si>
   <si>
     <t>PKIX_Test_28</t>
+  </si>
+  <si>
+    <t>2.16.840.1.101.3.6.6</t>
+  </si>
+  <si>
+    <t>1.3.6.1.1.16.4</t>
   </si>
 </sst>
 </file>
@@ -4073,7 +4079,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4260,6 +4266,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8347,8 +8362,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G464"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A329" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A350" sqref="A350:XFD350"/>
+    <sheetView topLeftCell="A398" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C427" sqref="C427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -19480,8 +19495,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:G29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -19996,12 +20011,11 @@
       <c r="D13" s="6" t="s">
         <v>1022</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="55" t="s">
+        <v>1265</v>
+      </c>
       <c r="F13" s="6" t="s">
         <v>759</v>
-      </c>
-      <c r="G13" s="55" t="s">
-        <v>1078</v>
       </c>
     </row>
     <row r="14" spans="1:256" ht="31.5" customHeight="1">
@@ -21521,39 +21535,43 @@
       <c r="IU27" s="35"/>
       <c r="IV27" s="35"/>
     </row>
-    <row r="28" spans="1:256" ht="60">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:256" ht="63">
+      <c r="A28" s="55" t="s">
         <v>1261</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="55" t="s">
         <v>999</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="55" t="s">
         <v>1263</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="52" t="s">
         <v>586</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:256" ht="30">
-      <c r="A29" s="57" t="s">
+      <c r="E28" s="66" t="s">
+        <v>1266</v>
+      </c>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="29" spans="1:256" ht="31.5">
+      <c r="A29" s="65" t="s">
         <v>1262</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="55" t="s">
         <v>999</v>
       </c>
       <c r="C29" s="55" t="s">
         <v>1264</v>
       </c>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="55" t="s">
         <v>588</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated databases with CMS changes
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D940C3C-9918-4917-80B1-D47257A13F7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67F48B7-E608-4F62-99E0-B62025A79A1B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17070" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="0" windowWidth="24000" windowHeight="16830" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="2" r:id="rId1"/>
@@ -3751,9 +3751,6 @@
     <t>Expiration Date is within the next 15 years</t>
   </si>
   <si>
-    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.248, X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID;2.16.840.1.101.3.2.1.48.251, X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID;2.16.840.1.101.3.2.1.48.250, X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.249, CARD_HOLDER_UNIQUE_IDENTIFIER_OID;2.16.840.1.101.3.2.1.48.252</t>
-  </si>
-  <si>
     <t>8.2.2.16</t>
   </si>
   <si>
@@ -3824,6 +3821,9 @@
   </si>
   <si>
     <t>OID for entryUUID</t>
+  </si>
+  <si>
+    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.248, X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID:2.16.840.1.101.3.2.1.48.251, X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID:2.16.840.1.101.3.2.1.48.250, X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.249, CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.2.1.48.252</t>
   </si>
 </sst>
 </file>
@@ -4640,7 +4640,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F473"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4682,7 +4682,7 @@
         <v>1196</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
@@ -5307,7 +5307,7 @@
         <v>54</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="C38" s="37" t="s">
         <v>719</v>
@@ -5934,7 +5934,7 @@
         <v>154</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="D74" s="37" t="s">
         <v>156</v>
@@ -5952,7 +5952,7 @@
         <v>157</v>
       </c>
       <c r="C75" s="39" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="D75" s="39" t="s">
         <v>1039</v>
@@ -5970,7 +5970,7 @@
         <v>160</v>
       </c>
       <c r="C76" s="39" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="D76" s="39" t="s">
         <v>1040</v>
@@ -5988,7 +5988,7 @@
         <v>163</v>
       </c>
       <c r="C77" s="37" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="D77" s="37" t="s">
         <v>159</v>
@@ -6006,7 +6006,7 @@
         <v>1041</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="D78" s="37" t="s">
         <v>162</v>
@@ -6024,7 +6024,7 @@
         <v>1042</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="D79" s="37" t="s">
         <v>165</v>
@@ -9696,7 +9696,7 @@
         <v>431</v>
       </c>
       <c r="C293" s="44" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="D293" s="37" t="s">
         <v>432</v>
@@ -10012,7 +10012,7 @@
         <v>449</v>
       </c>
       <c r="C311" s="44" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="D311" s="37" t="s">
         <v>432</v>
@@ -10514,7 +10514,7 @@
         <v>1080</v>
       </c>
       <c r="C340" s="44" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="D340" s="37" t="s">
         <v>432</v>
@@ -11568,7 +11568,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="403" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A403" s="38" t="s">
         <v>54</v>
       </c>
@@ -12162,7 +12162,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="438" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A438" s="38" t="s">
         <v>54</v>
       </c>
@@ -13252,7 +13252,7 @@
         <v>716</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>1237</v>
@@ -13750,7 +13750,7 @@
         <v>1084</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="E43" s="26"/>
       <c r="F43" s="4" t="s">
@@ -13769,7 +13769,7 @@
         <v>1085</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="E44" s="26"/>
       <c r="F44" s="4" t="s">
@@ -13788,7 +13788,7 @@
         <v>1086</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="E45" s="26"/>
       <c r="F45" s="4" t="s">
@@ -13807,7 +13807,7 @@
         <v>1087</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="4" t="s">
@@ -13826,7 +13826,7 @@
         <v>1088</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="E47" s="26"/>
       <c r="F47" s="4" t="s">
@@ -13845,7 +13845,7 @@
         <v>1089</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="E48" s="26"/>
       <c r="F48" s="4" t="s">
@@ -13864,7 +13864,7 @@
         <v>1090</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="4" t="s">
@@ -13883,7 +13883,7 @@
         <v>1091</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="E50" s="26"/>
       <c r="F50" s="4" t="s">
@@ -13902,7 +13902,7 @@
         <v>1092</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="E51" s="26"/>
       <c r="F51" s="4" t="s">
@@ -13921,7 +13921,7 @@
         <v>1093</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="4" t="s">
@@ -13940,7 +13940,7 @@
         <v>1094</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="E53" s="26"/>
       <c r="F53" s="4" t="s">
@@ -13959,7 +13959,7 @@
         <v>1095</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E54" s="26"/>
       <c r="F54" s="4" t="s">
@@ -17102,7 +17102,7 @@
         <v>685</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -17460,8 +17460,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17859,7 +17859,7 @@
         <v>1156</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>1239</v>
+        <v>1263</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>685</v>
@@ -18157,7 +18157,7 @@
         <v>963</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>703</v>

</xml_diff>

<commit_message>
Updated credential durations to be consistent between overview and 73-4
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C0FE48-0D31-4F3D-A432-9BDA64039A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC640F20-3F0D-455B-890A-609B01538831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2991" uniqueCount="1262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2991" uniqueCount="1261">
   <si>
     <t>Card Capabilities Container</t>
   </si>
@@ -3736,9 +3736,6 @@
     <t>digestAlgorithms field value of the SignedData is in accordance with Table 3-2 of SP 800-78.</t>
   </si>
   <si>
-    <t>CARD_HOLDER_UNIQUE_IDENTIFIER_OID:15</t>
-  </si>
-  <si>
     <t>Expiration Date is within the next 15 years</t>
   </si>
   <si>
@@ -3748,9 +3745,6 @@
     <t>BER-TLV Test Assertions</t>
   </si>
   <si>
-    <t>Expiration Date is within the next 5 years</t>
-  </si>
-  <si>
     <t>Printed Information Tags 0x01, 0x02, 0x05, 0x06 are present in that order</t>
   </si>
   <si>
@@ -3818,6 +3812,9 @@
   </si>
   <si>
     <t>CCC Tag 0xFE present and after any tags from 73-4.3 and 73-4.4</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -4678,7 +4675,7 @@
         <v>1193</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
@@ -4864,7 +4861,7 @@
         <v>77</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="D13" s="37" t="s">
         <v>78</v>
@@ -5303,7 +5300,7 @@
         <v>54</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="C38" s="37" t="s">
         <v>716</v>
@@ -5342,7 +5339,7 @@
         <v>111</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="D40" s="37" t="s">
         <v>112</v>
@@ -5930,7 +5927,7 @@
         <v>153</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="D74" s="37" t="s">
         <v>155</v>
@@ -5948,7 +5945,7 @@
         <v>156</v>
       </c>
       <c r="C75" s="39" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="D75" s="39" t="s">
         <v>1036</v>
@@ -5966,7 +5963,7 @@
         <v>159</v>
       </c>
       <c r="C76" s="39" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="D76" s="39" t="s">
         <v>1037</v>
@@ -5984,7 +5981,7 @@
         <v>162</v>
       </c>
       <c r="C77" s="37" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="D77" s="37" t="s">
         <v>158</v>
@@ -6002,7 +5999,7 @@
         <v>1038</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="D78" s="37" t="s">
         <v>161</v>
@@ -6020,7 +6017,7 @@
         <v>1039</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="D79" s="37" t="s">
         <v>164</v>
@@ -9692,7 +9689,7 @@
         <v>430</v>
       </c>
       <c r="C293" s="44" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="D293" s="37" t="s">
         <v>431</v>
@@ -10008,7 +10005,7 @@
         <v>448</v>
       </c>
       <c r="C311" s="44" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="D311" s="37" t="s">
         <v>431</v>
@@ -10510,7 +10507,7 @@
         <v>1077</v>
       </c>
       <c r="C340" s="44" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="D340" s="37" t="s">
         <v>431</v>
@@ -11192,7 +11189,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="381" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A381" s="38" t="s">
         <v>54</v>
       </c>
@@ -12912,7 +12909,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AMK56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13037,7 +13036,7 @@
         <v>698</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
@@ -13246,10 +13245,10 @@
         <v>713</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>1234</v>
+        <v>1260</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>683</v>
@@ -14762,7 +14761,7 @@
         <v>1081</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="E43" s="26"/>
       <c r="F43" s="4" t="s">
@@ -14781,7 +14780,7 @@
         <v>1082</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="E44" s="26"/>
       <c r="F44" s="4" t="s">
@@ -14800,7 +14799,7 @@
         <v>1083</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="E45" s="26"/>
       <c r="F45" s="4" t="s">
@@ -14819,7 +14818,7 @@
         <v>1084</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="4" t="s">
@@ -14838,7 +14837,7 @@
         <v>1085</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="E47" s="26"/>
       <c r="F47" s="4" t="s">
@@ -14857,7 +14856,7 @@
         <v>1086</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="E48" s="26"/>
       <c r="F48" s="4" t="s">
@@ -14876,7 +14875,7 @@
         <v>1087</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="4" t="s">
@@ -14895,7 +14894,7 @@
         <v>1088</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="E50" s="26"/>
       <c r="F50" s="4" t="s">
@@ -14914,7 +14913,7 @@
         <v>1089</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="E51" s="26"/>
       <c r="F51" s="4" t="s">
@@ -14933,7 +14932,7 @@
         <v>1090</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="4" t="s">
@@ -14952,7 +14951,7 @@
         <v>1091</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="E53" s="26"/>
       <c r="F53" s="4" t="s">
@@ -14971,7 +14970,7 @@
         <v>1092</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="E54" s="26"/>
       <c r="F54" s="4" t="s">
@@ -18114,7 +18113,7 @@
         <v>683</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -18472,7 +18471,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -18871,7 +18870,7 @@
         <v>1153</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>683</v>
@@ -19169,7 +19168,7 @@
         <v>960</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>700</v>

</xml_diff>

<commit_message>
Removed parameter to PKIX_20_Test()
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance-0.2.3-beta\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0DCB54-9B8C-44BB-9F83-DADAB774CF21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322461A8-779C-4D06-94A0-DEE942D72833}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="744" yWindow="1152" windowWidth="22296" windowHeight="12960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="336" windowWidth="22296" windowHeight="12960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3099" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3098" uniqueCount="1303">
   <si>
     <t>Document</t>
   </si>
@@ -3677,9 +3677,6 @@
   </si>
   <si>
     <t>PKIX_Test_24</t>
-  </si>
-  <si>
-    <t>2.5.29.31</t>
   </si>
   <si>
     <t>PKIX_Test_25</t>
@@ -4716,9 +4713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK490"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:F490"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5384,7 +5379,7 @@
         <v>6</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>884</v>
@@ -5492,10 +5487,10 @@
         <v>6</v>
       </c>
       <c r="B44" s="16" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>1233</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>1234</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -5975,7 +5970,7 @@
         <v>163</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>165</v>
@@ -5993,7 +5988,7 @@
         <v>166</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>167</v>
@@ -6234,7 +6229,7 @@
         <v>114</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="C87" s="16" t="s">
         <v>116</v>
@@ -6876,7 +6871,7 @@
         <v>6</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>237</v>
@@ -7312,7 +7307,7 @@
       </c>
       <c r="E149" s="16"/>
       <c r="F149" s="16" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -7330,7 +7325,7 @@
       </c>
       <c r="E150" s="16"/>
       <c r="F150" s="16" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -7348,7 +7343,7 @@
       </c>
       <c r="E151" s="16"/>
       <c r="F151" s="16" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -7384,7 +7379,7 @@
         <v>6</v>
       </c>
       <c r="B154" s="36" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="C154" s="10" t="s">
         <v>299</v>
@@ -7412,7 +7407,7 @@
         <v>6</v>
       </c>
       <c r="B156" s="16" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="C156" s="7" t="s">
         <v>302</v>
@@ -7724,10 +7719,10 @@
         <v>6</v>
       </c>
       <c r="B174" s="16" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C174" s="16" t="s">
         <v>1244</v>
-      </c>
-      <c r="C174" s="16" t="s">
-        <v>1245</v>
       </c>
       <c r="D174" s="16" t="s">
         <v>1073</v>
@@ -7760,7 +7755,7 @@
         <v>6</v>
       </c>
       <c r="B176" s="16" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="C176" s="14" t="s">
         <v>344</v>
@@ -7791,7 +7786,7 @@
         <v>347</v>
       </c>
       <c r="C178" s="16" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="D178" s="16">
         <v>76.099999999999994</v>
@@ -7827,7 +7822,7 @@
         <v>349</v>
       </c>
       <c r="C180" s="16" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="D180" s="16" t="s">
         <v>311</v>
@@ -8054,10 +8049,10 @@
         <v>6</v>
       </c>
       <c r="B193" s="16" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="C193" s="16" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="D193" s="16" t="s">
         <v>1073</v>
@@ -8121,7 +8116,7 @@
         <v>371</v>
       </c>
       <c r="C197" s="16" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="D197" s="16">
         <v>76.099999999999994</v>
@@ -8157,7 +8152,7 @@
         <v>374</v>
       </c>
       <c r="C199" s="16" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="D199" s="16" t="s">
         <v>311</v>
@@ -8384,10 +8379,10 @@
         <v>6</v>
       </c>
       <c r="B212" s="16" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="C212" s="16" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="D212" s="16" t="s">
         <v>1073</v>
@@ -8420,7 +8415,7 @@
         <v>6</v>
       </c>
       <c r="B214" s="16" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="C214" s="14" t="s">
         <v>394</v>
@@ -9206,7 +9201,7 @@
         <v>6</v>
       </c>
       <c r="B260" s="16" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="C260" s="7" t="s">
         <v>48</v>
@@ -9291,7 +9286,7 @@
         <v>501</v>
       </c>
       <c r="C265" s="15" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="D265" s="16" t="s">
         <v>502</v>
@@ -9392,7 +9387,7 @@
         <v>6</v>
       </c>
       <c r="B271" s="16" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="C271" s="15" t="s">
         <v>516</v>
@@ -9567,7 +9562,7 @@
         <v>538</v>
       </c>
       <c r="C281" s="15" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="D281" s="16" t="s">
         <v>502</v>
@@ -9779,7 +9774,7 @@
         <v>561</v>
       </c>
       <c r="C293" s="16" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D293" s="16" t="s">
         <v>563</v>
@@ -9797,7 +9792,7 @@
         <v>564</v>
       </c>
       <c r="C294" s="15" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="D294" s="16" t="s">
         <v>1144</v>
@@ -9812,7 +9807,7 @@
         <v>6</v>
       </c>
       <c r="B295" s="16" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="C295" s="15" t="s">
         <v>565</v>
@@ -9915,7 +9910,7 @@
         <v>574</v>
       </c>
       <c r="C301" s="15" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="D301" s="16" t="s">
         <v>502</v>
@@ -10002,7 +9997,7 @@
         <v>6</v>
       </c>
       <c r="B306" s="16" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="C306" s="10" t="s">
         <v>547</v>
@@ -10142,10 +10137,10 @@
         <v>6</v>
       </c>
       <c r="B314" s="16" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="C314" s="15" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="D314" s="16" t="s">
         <v>1144</v>
@@ -10467,7 +10462,7 @@
         <v>622</v>
       </c>
       <c r="C333" s="16" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="D333" s="16" t="s">
         <v>502</v>
@@ -10518,7 +10513,7 @@
         <v>6</v>
       </c>
       <c r="B336" s="16" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="C336" s="16" t="s">
         <v>542</v>
@@ -10536,7 +10531,7 @@
         <v>6</v>
       </c>
       <c r="B337" s="16" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="C337" s="16" t="s">
         <v>544</v>
@@ -10568,7 +10563,7 @@
         <v>6</v>
       </c>
       <c r="B339" s="16" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C339" s="16" t="s">
         <v>611</v>
@@ -10586,7 +10581,7 @@
         <v>6</v>
       </c>
       <c r="B340" s="16" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="C340" s="16" t="s">
         <v>552</v>
@@ -10697,7 +10692,7 @@
         <v>631</v>
       </c>
       <c r="C346" s="15" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="D346" s="16" t="s">
         <v>1144</v>
@@ -10744,7 +10739,7 @@
         <v>6</v>
       </c>
       <c r="B349" s="16" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="C349" s="10" t="s">
         <v>635</v>
@@ -10840,7 +10835,7 @@
         <v>6</v>
       </c>
       <c r="B355" s="16" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C355" s="10" t="s">
         <v>711</v>
@@ -10890,7 +10885,7 @@
         <v>6</v>
       </c>
       <c r="B358" s="16" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C358" s="15" t="s">
         <v>650</v>
@@ -10908,7 +10903,7 @@
         <v>6</v>
       </c>
       <c r="B359" s="16" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C359" s="16" t="s">
         <v>653</v>
@@ -10996,7 +10991,7 @@
         <v>665</v>
       </c>
       <c r="C364" s="40" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="D364" s="40" t="s">
         <v>685</v>
@@ -11010,10 +11005,10 @@
         <v>6</v>
       </c>
       <c r="B365" s="41" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C365" s="41" t="s">
         <v>1286</v>
-      </c>
-      <c r="C365" s="41" t="s">
-        <v>1287</v>
       </c>
       <c r="D365" s="41" t="s">
         <v>666</v>
@@ -11027,10 +11022,10 @@
         <v>6</v>
       </c>
       <c r="B366" s="16" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C366" s="15" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="D366" s="16"/>
       <c r="E366" s="16"/>
@@ -11073,10 +11068,10 @@
         <v>6</v>
       </c>
       <c r="B369" s="16" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C369" s="15" t="s">
         <v>1270</v>
-      </c>
-      <c r="C369" s="15" t="s">
-        <v>1271</v>
       </c>
       <c r="D369" s="16" t="s">
         <v>1182</v>
@@ -11162,10 +11157,10 @@
         <v>683</v>
       </c>
       <c r="C374" s="43" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D374" s="42" t="s">
         <v>1288</v>
-      </c>
-      <c r="D374" s="42" t="s">
-        <v>1289</v>
       </c>
       <c r="E374" s="42"/>
       <c r="F374" s="42" t="s">
@@ -12266,10 +12261,10 @@
         <v>695</v>
       </c>
       <c r="C379" s="40" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D379" s="40" t="s">
         <v>1290</v>
-      </c>
-      <c r="D379" s="40" t="s">
-        <v>1291</v>
       </c>
       <c r="F379" s="40" t="s">
         <v>119</v>
@@ -12283,10 +12278,10 @@
         <v>696</v>
       </c>
       <c r="C380" s="41" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D380" s="41" t="s">
         <v>1292</v>
-      </c>
-      <c r="D380" s="41" t="s">
-        <v>1293</v>
       </c>
       <c r="F380" s="41" t="s">
         <v>119</v>
@@ -12315,7 +12310,7 @@
         <v>6</v>
       </c>
       <c r="B382" s="16" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="C382" s="7" t="s">
         <v>700</v>
@@ -12461,7 +12456,7 @@
         <v>6</v>
       </c>
       <c r="B391" s="16" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="C391" s="15" t="s">
         <v>749</v>
@@ -13587,10 +13582,10 @@
         <v>726</v>
       </c>
       <c r="C397" s="42" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D397" s="42" t="s">
         <v>1288</v>
-      </c>
-      <c r="D397" s="42" t="s">
-        <v>1289</v>
       </c>
       <c r="F397" s="42" t="s">
         <v>196</v>
@@ -16728,10 +16723,10 @@
         <v>731</v>
       </c>
       <c r="C402" s="40" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D402" s="40" t="s">
         <v>1290</v>
-      </c>
-      <c r="D402" s="40" t="s">
-        <v>1291</v>
       </c>
       <c r="F402" s="40" t="s">
         <v>196</v>
@@ -16745,10 +16740,10 @@
         <v>732</v>
       </c>
       <c r="C403" s="41" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D403" s="41" t="s">
         <v>1292</v>
-      </c>
-      <c r="D403" s="41" t="s">
-        <v>1293</v>
       </c>
       <c r="F403" s="41" t="s">
         <v>196</v>
@@ -17796,7 +17791,7 @@
         <v>6</v>
       </c>
       <c r="B405" s="16" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C405" s="7" t="s">
         <v>734</v>
@@ -17924,7 +17919,7 @@
         <v>6</v>
       </c>
       <c r="B413" s="16" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C413" s="15" t="s">
         <v>745</v>
@@ -17942,7 +17937,7 @@
         <v>6</v>
       </c>
       <c r="B414" s="16" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="C414" s="15" t="s">
         <v>747</v>
@@ -17960,7 +17955,7 @@
         <v>6</v>
       </c>
       <c r="B415" s="16" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C415" s="15" t="s">
         <v>749</v>
@@ -19071,7 +19066,7 @@
         <v>684</v>
       </c>
       <c r="D420" s="42" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="F420" s="42" t="s">
         <v>211</v>
@@ -22209,10 +22204,10 @@
         <v>761</v>
       </c>
       <c r="C425" s="40" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D425" s="40" t="s">
         <v>1290</v>
-      </c>
-      <c r="D425" s="40" t="s">
-        <v>1291</v>
       </c>
       <c r="F425" s="40" t="s">
         <v>211</v>
@@ -22226,10 +22221,10 @@
         <v>762</v>
       </c>
       <c r="C426" s="41" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D426" s="41" t="s">
         <v>1292</v>
-      </c>
-      <c r="D426" s="41" t="s">
-        <v>1293</v>
       </c>
       <c r="F426" s="41" t="s">
         <v>211</v>
@@ -22258,7 +22253,7 @@
         <v>6</v>
       </c>
       <c r="B428" s="16" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="C428" s="7" t="s">
         <v>764</v>
@@ -22560,10 +22555,10 @@
         <v>792</v>
       </c>
       <c r="C446" s="40" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D446" s="40" t="s">
         <v>1290</v>
-      </c>
-      <c r="D446" s="40" t="s">
-        <v>1291</v>
       </c>
       <c r="F446" s="40" t="s">
         <v>226</v>
@@ -22577,10 +22572,10 @@
         <v>793</v>
       </c>
       <c r="C447" s="41" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D447" s="41" t="s">
         <v>1292</v>
-      </c>
-      <c r="D447" s="41" t="s">
-        <v>1293</v>
       </c>
       <c r="F447" s="41" t="s">
         <v>226</v>
@@ -22591,10 +22586,10 @@
         <v>6</v>
       </c>
       <c r="B448" s="16" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="C448" s="15" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="D448" s="16"/>
       <c r="E448" s="15"/>
@@ -22637,10 +22632,10 @@
         <v>6</v>
       </c>
       <c r="B451" s="16" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="C451" s="15" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="D451" s="16" t="s">
         <v>1182</v>
@@ -22726,10 +22721,10 @@
         <v>802</v>
       </c>
       <c r="C456" s="42" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D456" s="42" t="s">
         <v>1288</v>
-      </c>
-      <c r="D456" s="42" t="s">
-        <v>1289</v>
       </c>
       <c r="F456" s="42" t="s">
         <v>226</v>
@@ -23809,7 +23804,7 @@
         <v>6</v>
       </c>
       <c r="B460" s="16" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="C460" s="7" t="s">
         <v>807</v>
@@ -23865,7 +23860,7 @@
         <v>6</v>
       </c>
       <c r="B464" s="16" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="C464" s="7" t="s">
         <v>812</v>
@@ -23907,7 +23902,7 @@
         <v>6</v>
       </c>
       <c r="B467" s="16" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="C467" s="7" t="s">
         <v>816</v>
@@ -24053,7 +24048,7 @@
         <v>6</v>
       </c>
       <c r="B476" s="16" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C476" s="15" t="s">
         <v>776</v>
@@ -24176,10 +24171,10 @@
         <v>838</v>
       </c>
       <c r="C483" s="42" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D483" s="42" t="s">
         <v>1288</v>
-      </c>
-      <c r="D483" s="42" t="s">
-        <v>1289</v>
       </c>
       <c r="F483" s="42" t="s">
         <v>51</v>
@@ -25279,10 +25274,10 @@
         <v>843</v>
       </c>
       <c r="C488" s="40" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D488" s="40" t="s">
         <v>1290</v>
-      </c>
-      <c r="D488" s="40" t="s">
-        <v>1291</v>
       </c>
       <c r="F488" s="40" t="s">
         <v>51</v>
@@ -25296,10 +25291,10 @@
         <v>844</v>
       </c>
       <c r="C489" s="41" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D489" s="41" t="s">
         <v>1292</v>
-      </c>
-      <c r="D489" s="41" t="s">
-        <v>1293</v>
       </c>
       <c r="F489" s="41" t="s">
         <v>51</v>
@@ -29000,9 +28995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMK32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -29419,7 +29412,7 @@
         <v>1175</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="47" t="s">
@@ -29457,7 +29450,7 @@
         <v>1177</v>
       </c>
       <c r="D10" s="56" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="47" t="s">
@@ -29985,7 +29978,7 @@
         <v>1213</v>
       </c>
       <c r="D24" s="47" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="E24" s="47"/>
       <c r="F24" s="47" t="s">
@@ -30255,9 +30248,7 @@
       <c r="D25" s="47" t="s">
         <v>687</v>
       </c>
-      <c r="E25" s="47" t="s">
-        <v>1215</v>
-      </c>
+      <c r="E25" s="47"/>
       <c r="F25" s="47" t="s">
         <v>856</v>
       </c>
@@ -30520,7 +30511,7 @@
         <v>1160</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="D26" s="47" t="s">
         <v>698</v>
@@ -30788,7 +30779,7 @@
         <v>1160</v>
       </c>
       <c r="C27" s="55" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="D27" s="47" t="s">
         <v>827</v>
@@ -31056,7 +31047,7 @@
         <v>1160</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="D28" s="47" t="s">
         <v>673</v>
@@ -31068,7 +31059,7 @@
         <v>856</v>
       </c>
       <c r="G28" s="55" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="29" spans="1:256" ht="31.2" x14ac:dyDescent="0.3">
@@ -31079,10 +31070,10 @@
         <v>1160</v>
       </c>
       <c r="C29" s="47" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D29" s="47" t="s">
         <v>1220</v>
-      </c>
-      <c r="D29" s="47" t="s">
-        <v>1221</v>
       </c>
       <c r="E29" s="47"/>
       <c r="F29" s="47" t="s">
@@ -31092,16 +31083,16 @@
     </row>
     <row r="30" spans="1:256" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A30" s="56" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="B30" s="47" t="s">
         <v>1160</v>
       </c>
       <c r="C30" s="56" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D30" s="56" t="s">
         <v>1298</v>
-      </c>
-      <c r="D30" s="56" t="s">
-        <v>1299</v>
       </c>
       <c r="E30" s="47"/>
       <c r="F30" s="47" t="s">
@@ -31111,16 +31102,16 @@
     </row>
     <row r="31" spans="1:256" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A31" s="56" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="B31" s="47" t="s">
         <v>1160</v>
       </c>
       <c r="C31" s="56" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D31" s="56" t="s">
         <v>1300</v>
-      </c>
-      <c r="D31" s="56" t="s">
-        <v>1301</v>
       </c>
       <c r="E31" s="55"/>
       <c r="F31" s="47" t="s">
@@ -31130,16 +31121,16 @@
     </row>
     <row r="32" spans="1:256" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="56" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B32" s="47" t="s">
         <v>1160</v>
       </c>
       <c r="C32" s="56" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D32" s="56" t="s">
         <v>1302</v>
-      </c>
-      <c r="D32" s="56" t="s">
-        <v>1303</v>
       </c>
       <c r="E32" s="55"/>
       <c r="F32" s="47" t="s">
@@ -31450,37 +31441,37 @@
         <v>278</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>1222</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>1223</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>1224</v>
       </c>
       <c r="E2" s="18"/>
       <c r="F2" s="18" t="s">
         <v>856</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="3" spans="1:256" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>1226</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>1222</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="18" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>1227</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>1224</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>1228</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>872</v>
@@ -31489,19 +31480,19 @@
     </row>
     <row r="4" spans="1:256" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>1229</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>1222</v>
-      </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>1230</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>1224</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>1231</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>872</v>

</xml_diff>

<commit_message>
Disabled PIV-specific test cases
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance-0.2.3-beta\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322461A8-779C-4D06-94A0-DEE942D72833}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4A9A54-0DBF-41B2-A5DD-B2A45AB6A5D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="336" windowWidth="22296" windowHeight="12960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3098" uniqueCount="1303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3096" uniqueCount="1304">
   <si>
     <t>Document</t>
   </si>
@@ -3941,6 +3941,9 @@
   </si>
   <si>
     <t>The URI scheme for id-ce-cRLDistributionPoints is "http" (not "https")</t>
+  </si>
+  <si>
+    <t>Not tested for PIV-I. GeneralName field exists that contains an otherName with a type-id asserting the pivFASC-N OID. The value field of this otherName contains the FASC-N for the cardholder which matches the FASC-N obtained from parsing the CHUID.</t>
   </si>
 </sst>
 </file>
@@ -4713,7 +4716,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK490"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A353" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A369" sqref="A369"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11071,15 +11076,11 @@
         <v>1269</v>
       </c>
       <c r="C369" s="15" t="s">
-        <v>1270</v>
-      </c>
-      <c r="D369" s="16" t="s">
-        <v>1182</v>
-      </c>
+        <v>1303</v>
+      </c>
+      <c r="D369" s="16"/>
       <c r="E369" s="15"/>
-      <c r="F369" s="16" t="s">
-        <v>119</v>
-      </c>
+      <c r="F369" s="16"/>
     </row>
     <row r="370" spans="1:1025" ht="45" x14ac:dyDescent="0.3">
       <c r="A370" s="16" t="s">
@@ -28995,7 +28996,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMK32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Corrected 8.5.1.5 test description
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DD5A97-B991-46C3-A316-8817FBDDCA8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC433F76-ABF2-426F-A26B-16AB33EB32BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="48" windowWidth="17280" windowHeight="13416" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3087" uniqueCount="1310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3087" uniqueCount="1311">
   <si>
     <t>Document</t>
   </si>
@@ -3962,6 +3962,9 @@
   </si>
   <si>
     <t>File has an extension of “.p7c” containing a certs-only CMS message (see RFC 3851)</t>
+  </si>
+  <si>
+    <t>No tags other than (0x01, 0x02, 0x04, 0x05, 0x06, 0x07, 0x08, 0xFE) are present</t>
   </si>
 </sst>
 </file>
@@ -4746,9 +4749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A376" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C381" sqref="C381"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6067,7 +6068,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A76" s="16" t="s">
         <v>6</v>
       </c>
@@ -6075,7 +6076,7 @@
         <v>171</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>910</v>
+        <v>1310</v>
       </c>
       <c r="D76" s="16" t="s">
         <v>172</v>
@@ -27016,8 +27017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView showGridLines="0" topLeftCell="B25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>